<commit_message>
test case 2 passed
</commit_message>
<xml_diff>
--- a/com.freecrm/src/test/resources/test_data_freecrm.xlsx
+++ b/com.freecrm/src/test/resources/test_data_freecrm.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.freecrm/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D5C75C-696C-F347-A36F-1798D38A093F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84AA51B-10EB-BC41-9F1D-DEEC035F3A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="1" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateNewCompany" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -45,6 +46,48 @@
   </si>
   <si>
     <t>Adil Khaleque</t>
+  </si>
+  <si>
+    <t>Company1</t>
+  </si>
+  <si>
+    <t>1234 56th St</t>
+  </si>
+  <si>
+    <t>New York City, NY</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>My First Company.</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2111111111</t>
+  </si>
+  <si>
+    <t>Mobile</t>
   </si>
 </sst>
 </file>
@@ -89,9 +132,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -409,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9FA16C-0ECE-414F-A530-A2D72F14E475}">
   <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,4 +481,91 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE64F308-C8DB-D340-814A-BA5743B66477}">
+  <dimension ref="A2:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="17.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.5" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{7EA26A1D-F7D1-244D-B215-F12DFA57F273}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test case 3 passed
</commit_message>
<xml_diff>
--- a/com.freecrm/src/test/resources/test_data_freecrm.xlsx
+++ b/com.freecrm/src/test/resources/test_data_freecrm.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.freecrm/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9815012-16B3-9A4D-B813-F6DB7FC09707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E38300B-DCB8-FC44-A8D4-F6E9A80F550C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="1" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="2" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
     <sheet name="CreateNewCompany" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateNewContact" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -88,6 +89,48 @@
   </si>
   <si>
     <t>New York City</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>11 Hydrant St</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>12121</t>
+  </si>
+  <si>
+    <t>Simon Winter</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>New contact for Company1.</t>
   </si>
 </sst>
 </file>
@@ -132,10 +175,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -487,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE64F308-C8DB-D340-814A-BA5743B66477}">
   <dimension ref="A2:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,4 +612,114 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7204117C-D6A3-4146-A764-7DAF36603B13}">
+  <dimension ref="A2:X2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="10.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.83203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="27" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" style="2" customWidth="1"/>
+    <col min="14" max="23" width="10.83203125" style="2"/>
+    <col min="24" max="24" width="12.5" style="2" customWidth="1"/>
+    <col min="25" max="25" width="14" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F1A476BF-04C7-1E4A-9332-28AF95298610}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{34A51966-4422-9542-9A60-224D71C69AC6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test case 6 passed
</commit_message>
<xml_diff>
--- a/com.freecrm/src/test/resources/test_data_freecrm.xlsx
+++ b/com.freecrm/src/test/resources/test_data_freecrm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.freecrm/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2490274B-D81E-184F-9A26-05315861C800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0011939C-12DD-BC43-9B4A-ABABAD59E67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="4" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="5" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="CreateNewContact" sheetId="3" r:id="rId3"/>
     <sheet name="CreateNewDeal" sheetId="4" r:id="rId4"/>
     <sheet name="CreateNewCase" sheetId="5" r:id="rId5"/>
+    <sheet name="CreateNewTask" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -172,6 +173,21 @@
   </si>
   <si>
     <t>Case1 includes Deal1 for Company1 to Simon Winter and is reffered to Adil Khaleque.</t>
+  </si>
+  <si>
+    <t>Task1</t>
+  </si>
+  <si>
+    <t>26/12/2022 09:00</t>
+  </si>
+  <si>
+    <t>30/12/2022 09:00</t>
+  </si>
+  <si>
+    <t>Due date on the 26th with a close date on the 30th</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -860,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FEF5B8-D9F7-2641-9492-D735ECA94236}">
   <dimension ref="A2:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -928,4 +944,80 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4559044C-52B7-614C-979D-9116671B560F}">
+  <dimension ref="A2:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="17.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13" style="2" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="2"/>
+    <col min="10" max="10" width="16.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="43.33203125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{217E5714-9DB1-8044-BC71-AAAFD6F20537}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test case 7 passed
</commit_message>
<xml_diff>
--- a/com.freecrm/src/test/resources/test_data_freecrm.xlsx
+++ b/com.freecrm/src/test/resources/test_data_freecrm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.freecrm/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0011939C-12DD-BC43-9B4A-ABABAD59E67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED65E62A-25AE-634C-AA86-4DAE4467EAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="5" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="6" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="CreateNewDeal" sheetId="4" r:id="rId4"/>
     <sheet name="CreateNewCase" sheetId="5" r:id="rId5"/>
     <sheet name="CreateNewTask" sheetId="6" r:id="rId6"/>
+    <sheet name="CreateNewCall" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="54">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -188,13 +189,28 @@
   </si>
   <si>
     <t>100</t>
+  </si>
+  <si>
+    <t>02/01/2022 09:00</t>
+  </si>
+  <si>
+    <t>30m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 30 min call to go over some important stuff. </t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>Simon Winter [Mobile +12111111111]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -206,6 +222,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -232,11 +254,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -950,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4559044C-52B7-614C-979D-9116671B560F}">
   <dimension ref="A2:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1020,4 +1043,86 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0A64E2-2E76-6246-B415-32265EAFA027}">
+  <dimension ref="A2:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="17" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="40" style="2" customWidth="1"/>
+    <col min="10" max="10" width="32.33203125" style="2" customWidth="1"/>
+    <col min="11" max="15" width="10.83203125" style="2"/>
+    <col min="16" max="16" width="15.83203125" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{A62DC227-63D7-BF42-BCD1-9CE9C50B7546}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test case new document passed
</commit_message>
<xml_diff>
--- a/com.freecrm/src/test/resources/test_data_freecrm.xlsx
+++ b/com.freecrm/src/test/resources/test_data_freecrm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.freecrm/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED65E62A-25AE-634C-AA86-4DAE4467EAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545A49EA-AD8E-CF4B-9418-A31ACABB69BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="6" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="7" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="CreateNewCase" sheetId="5" r:id="rId5"/>
     <sheet name="CreateNewTask" sheetId="6" r:id="rId6"/>
     <sheet name="CreateNewCall" sheetId="7" r:id="rId7"/>
+    <sheet name="CreateNewDocument" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="55">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -203,7 +204,10 @@
     <t>Work</t>
   </si>
   <si>
-    <t>Simon Winter [Mobile +12111111111]</t>
+    <t>Document1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is document1. </t>
   </si>
 </sst>
 </file>
@@ -1049,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0A64E2-2E76-6246-B415-32265EAFA027}">
   <dimension ref="A2:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1063,7 +1067,7 @@
     <col min="7" max="7" width="17" style="2" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="2"/>
     <col min="9" max="9" width="40" style="2" customWidth="1"/>
-    <col min="10" max="10" width="32.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" style="2" customWidth="1"/>
     <col min="11" max="15" width="10.83203125" style="2"/>
     <col min="16" max="16" width="15.83203125" style="2" customWidth="1"/>
     <col min="17" max="16384" width="10.83203125" style="2"/>
@@ -1098,7 +1102,7 @@
         <v>51</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>31</v>
@@ -1125,4 +1129,60 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCABBD67-C4D4-3C48-80E7-79AC6ED30147}">
+  <dimension ref="A2:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{FE148A77-90C8-D24A-A091-89A2464947CA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test create new campaign passed
</commit_message>
<xml_diff>
--- a/com.freecrm/src/test/resources/test_data_freecrm.xlsx
+++ b/com.freecrm/src/test/resources/test_data_freecrm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.freecrm/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545A49EA-AD8E-CF4B-9418-A31ACABB69BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A456DD2-7381-574B-8B27-440C7FC00FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="7" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="8" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="CreateNewTask" sheetId="6" r:id="rId6"/>
     <sheet name="CreateNewCall" sheetId="7" r:id="rId7"/>
     <sheet name="CreateNewDocument" sheetId="8" r:id="rId8"/>
+    <sheet name="CreateNewCampaign" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -208,6 +209,12 @@
   </si>
   <si>
     <t xml:space="preserve">This is document1. </t>
+  </si>
+  <si>
+    <t>Campaign1</t>
+  </si>
+  <si>
+    <t>Campaign1 [Active]</t>
   </si>
 </sst>
 </file>
@@ -1135,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCABBD67-C4D4-3C48-80E7-79AC6ED30147}">
   <dimension ref="A2:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1185,4 +1192,46 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C485ECE-8324-BD4F-AB82-9B760BC405FC}">
+  <dimension ref="A2:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="18" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{A1A7473B-A58C-9C4E-B935-A591AACA4EC2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test case create new event passed
</commit_message>
<xml_diff>
--- a/com.freecrm/src/test/resources/test_data_freecrm.xlsx
+++ b/com.freecrm/src/test/resources/test_data_freecrm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.freecrm/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A456DD2-7381-574B-8B27-440C7FC00FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC55160-634D-4E47-B14F-1153A4BCBD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="8" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" firstSheet="1" activeTab="9" xr2:uid="{8CC32EED-2BF6-7649-9115-210B71963079}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="CreateNewCall" sheetId="7" r:id="rId7"/>
     <sheet name="CreateNewDocument" sheetId="8" r:id="rId8"/>
     <sheet name="CreateNewCampaign" sheetId="9" r:id="rId9"/>
+    <sheet name="CreateNewEvent" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="63">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -215,6 +216,24 @@
   </si>
   <si>
     <t>Campaign1 [Active]</t>
+  </si>
+  <si>
+    <t>Event1</t>
+  </si>
+  <si>
+    <t>02/01/2022 08:00</t>
+  </si>
+  <si>
+    <t>02/01/2022 08:30</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>This event includes Deal1, Task1, and Case1.</t>
+  </si>
+  <si>
+    <t>New York, NY</t>
   </si>
 </sst>
 </file>
@@ -618,6 +637,85 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC2C9D6-AC9E-2F4B-9112-AFDB150AC627}">
+  <dimension ref="A2:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="16.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="37.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3F9A97B0-BEBB-8D44-9100-CAC000A6EF60}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE64F308-C8DB-D340-814A-BA5743B66477}">
   <dimension ref="A2:R2"/>
@@ -1198,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C485ECE-8324-BD4F-AB82-9B760BC405FC}">
   <dimension ref="A2:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>